<commit_message>
Add more result other pc
</commit_message>
<xml_diff>
--- a/misc/calibrator_results/calibrator_results.xlsx
+++ b/misc/calibrator_results/calibrator_results.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\halite3\misc\calibrator_results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{692AD5CD-F82C-4041-963C-C6F3E04E5A0E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9096" xr2:uid="{1ED4B686-DF9C-449E-8484-1D2AD312234D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9090"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$1</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="9">
   <si>
     <t>param</t>
   </si>
@@ -60,7 +59,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -404,20 +403,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27C34AD4-08EB-4F2D-849C-2A7825015302}">
-  <dimension ref="A1:F11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -437,7 +436,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -457,7 +456,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -477,7 +476,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -497,7 +496,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -517,7 +516,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -537,7 +536,7 @@
         <v>15.95</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -557,7 +556,7 @@
         <v>7.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -577,7 +576,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -597,7 +596,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -617,7 +616,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -637,8 +636,28 @@
         <v>0.02</v>
       </c>
     </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="C12">
+        <v>48</v>
+      </c>
+      <c r="D12">
+        <v>7</v>
+      </c>
+      <c r="E12">
+        <v>0.43</v>
+      </c>
+      <c r="F12">
+        <v>0.08</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:F1" xr:uid="{36B06730-5F39-4EF1-B096-4F4C86682C15}">
+  <autoFilter ref="A1:F1">
     <sortState ref="A2:F11">
       <sortCondition ref="A1"/>
     </sortState>

</xml_diff>

<commit_message>
Update training results overview
</commit_message>
<xml_diff>
--- a/misc/calibrator_results/calibrator_results.xlsx
+++ b/misc/calibrator_results/calibrator_results.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\halite3\misc\calibrator_results\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{FF7B8ED7-D5D8-46DE-B20C-011D8EED6156}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9090"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9096" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$1</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="16">
   <si>
     <t>param</t>
   </si>
@@ -54,12 +55,33 @@
   </si>
   <si>
     <t>mean_halite</t>
+  </si>
+  <si>
+    <t>expand_edge_cost</t>
+  </si>
+  <si>
+    <t>return_factor</t>
+  </si>
+  <si>
+    <t>neighbour_profit_factor</t>
+  </si>
+  <si>
+    <t>return_distance_factor</t>
+  </si>
+  <si>
+    <t>upload</t>
+  </si>
+  <si>
+    <t>jonne</t>
+  </si>
+  <si>
+    <t>stefan</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -403,20 +425,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -435,230 +457,545 @@
       <c r="F1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>40</v>
+      </c>
+      <c r="D2">
+        <v>6</v>
+      </c>
+      <c r="E2">
+        <v>2.93</v>
+      </c>
+      <c r="F2">
+        <f>0.95*0.8</f>
+        <v>0.76</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>40</v>
+      </c>
+      <c r="D3">
+        <v>11</v>
+      </c>
+      <c r="E3">
+        <v>2.5480700379946</v>
+      </c>
+      <c r="F3">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>32</v>
+      </c>
+      <c r="D4">
+        <v>6</v>
+      </c>
+      <c r="E4">
+        <v>3.22</v>
+      </c>
+      <c r="F4">
+        <v>0.44</v>
+      </c>
+      <c r="G4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="B2">
-        <v>2</v>
-      </c>
-      <c r="C2">
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
         <v>32</v>
-      </c>
-      <c r="D2">
-        <v>20</v>
-      </c>
-      <c r="E2">
-        <v>0.66</v>
-      </c>
-      <c r="F2">
-        <v>3.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>40</v>
-      </c>
-      <c r="D3">
-        <v>20</v>
-      </c>
-      <c r="E3">
-        <v>0.81</v>
-      </c>
-      <c r="F3">
-        <v>4.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4">
-        <v>4</v>
-      </c>
-      <c r="C4">
-        <v>40</v>
-      </c>
-      <c r="D4">
-        <v>14</v>
-      </c>
-      <c r="E4">
-        <v>0.27</v>
-      </c>
-      <c r="F4">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
-      <c r="C5">
-        <v>48</v>
       </c>
       <c r="D5">
         <v>20</v>
       </c>
       <c r="E5">
-        <v>146.78</v>
+        <v>0.66</v>
       </c>
       <c r="F5">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="G5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>40</v>
+      </c>
+      <c r="D6">
+        <v>20</v>
+      </c>
+      <c r="E6">
+        <v>0.81</v>
+      </c>
+      <c r="F6">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="G6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7">
+        <v>40</v>
+      </c>
+      <c r="D7">
+        <v>14</v>
+      </c>
+      <c r="E7">
+        <v>0.27</v>
+      </c>
+      <c r="F7">
+        <v>0.01</v>
+      </c>
+      <c r="G7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="B6">
-        <v>4</v>
-      </c>
-      <c r="C6">
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8">
         <v>48</v>
-      </c>
-      <c r="D6">
-        <v>10</v>
-      </c>
-      <c r="E6">
-        <v>159</v>
-      </c>
-      <c r="F6">
-        <v>15.95</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7">
-        <v>2</v>
-      </c>
-      <c r="C7">
-        <v>32</v>
-      </c>
-      <c r="D7">
-        <v>20</v>
-      </c>
-      <c r="E7">
-        <v>1.42</v>
-      </c>
-      <c r="F7">
-        <v>7.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8">
-        <v>2</v>
-      </c>
-      <c r="C8">
-        <v>40</v>
       </c>
       <c r="D8">
         <v>20</v>
       </c>
       <c r="E8">
-        <v>0.71</v>
+        <v>146.78</v>
       </c>
       <c r="F8">
-        <v>3.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0.7</v>
+      </c>
+      <c r="G8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B9">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C9">
         <v>48</v>
       </c>
       <c r="D9">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E9">
-        <v>0.72</v>
+        <v>159</v>
       </c>
       <c r="F9">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+        <v>15.95</v>
+      </c>
+      <c r="G9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B10">
         <v>4</v>
       </c>
       <c r="C10">
+        <v>40</v>
+      </c>
+      <c r="D10">
+        <v>6</v>
+      </c>
+      <c r="E10">
+        <v>2.29</v>
+      </c>
+      <c r="F10">
+        <f>0.56*0.8</f>
+        <v>0.44800000000000006</v>
+      </c>
+      <c r="G10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>40</v>
+      </c>
+      <c r="D11">
+        <v>11</v>
+      </c>
+      <c r="E11">
+        <v>1.87</v>
+      </c>
+      <c r="F11">
+        <v>0.05</v>
+      </c>
+      <c r="G11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
         <v>32</v>
       </c>
-      <c r="D10">
+      <c r="D12">
+        <v>6</v>
+      </c>
+      <c r="E12">
+        <v>3.96</v>
+      </c>
+      <c r="F12">
+        <v>0.54</v>
+      </c>
+      <c r="G12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>4</v>
+      </c>
+      <c r="C13">
+        <v>40</v>
+      </c>
+      <c r="D13">
+        <v>6</v>
+      </c>
+      <c r="E13">
+        <v>0.37</v>
+      </c>
+      <c r="F13">
+        <f>0.11*0.8</f>
+        <v>8.8000000000000009E-2</v>
+      </c>
+      <c r="G13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14">
+        <v>40</v>
+      </c>
+      <c r="D14">
         <v>11</v>
       </c>
-      <c r="E10">
+      <c r="E14">
+        <v>0.77</v>
+      </c>
+      <c r="F14">
+        <v>0.02</v>
+      </c>
+      <c r="G14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15">
+        <v>32</v>
+      </c>
+      <c r="D15">
+        <v>6</v>
+      </c>
+      <c r="E15">
+        <v>0.71</v>
+      </c>
+      <c r="F15">
+        <v>0.08</v>
+      </c>
+      <c r="G15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16">
+        <v>4</v>
+      </c>
+      <c r="C16">
+        <v>40</v>
+      </c>
+      <c r="D16">
+        <v>6</v>
+      </c>
+      <c r="E16">
+        <v>0.71</v>
+      </c>
+      <c r="F16">
+        <v>0.17</v>
+      </c>
+      <c r="G16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17">
+        <v>40</v>
+      </c>
+      <c r="D17">
+        <v>11</v>
+      </c>
+      <c r="E17">
+        <v>0.69</v>
+      </c>
+      <c r="F17">
+        <v>0.02</v>
+      </c>
+      <c r="G17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18">
+        <v>32</v>
+      </c>
+      <c r="D18">
+        <v>6</v>
+      </c>
+      <c r="E18">
+        <v>1.26</v>
+      </c>
+      <c r="F18">
+        <v>0.17</v>
+      </c>
+      <c r="G18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19">
+        <v>32</v>
+      </c>
+      <c r="D19">
+        <v>20</v>
+      </c>
+      <c r="E19">
+        <v>1.42</v>
+      </c>
+      <c r="F19">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="G19" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20">
+        <v>40</v>
+      </c>
+      <c r="D20">
+        <v>20</v>
+      </c>
+      <c r="E20">
+        <v>0.71</v>
+      </c>
+      <c r="F20">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="G20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21">
+        <v>48</v>
+      </c>
+      <c r="D21">
+        <v>7</v>
+      </c>
+      <c r="E21">
+        <v>0.72</v>
+      </c>
+      <c r="F21">
+        <v>0.05</v>
+      </c>
+      <c r="G21" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22">
+        <v>4</v>
+      </c>
+      <c r="C22">
+        <v>32</v>
+      </c>
+      <c r="D22">
+        <v>11</v>
+      </c>
+      <c r="E22">
         <v>1.24</v>
       </c>
-      <c r="F10">
+      <c r="F22">
         <v>0.09</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="G22" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>5</v>
       </c>
-      <c r="B11">
+      <c r="B23">
         <v>4</v>
       </c>
-      <c r="C11">
-        <v>40</v>
-      </c>
-      <c r="D11">
+      <c r="C23">
+        <v>40</v>
+      </c>
+      <c r="D23">
         <v>17</v>
       </c>
-      <c r="E11">
+      <c r="E23">
         <v>1.27</v>
       </c>
-      <c r="F11">
+      <c r="F23">
         <v>0.02</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="G23" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>5</v>
       </c>
-      <c r="B12">
+      <c r="B24">
         <v>4</v>
       </c>
-      <c r="C12">
+      <c r="C24">
         <v>48</v>
       </c>
-      <c r="D12">
+      <c r="D24">
         <v>7</v>
       </c>
-      <c r="E12">
+      <c r="E24">
         <v>0.43</v>
       </c>
-      <c r="F12">
+      <c r="F24">
         <v>0.08</v>
       </c>
+      <c r="G24" t="s">
+        <v>14</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F1">
-    <sortState ref="A2:F11">
+  <autoFilter ref="A1:G1" xr:uid="{C635C791-9EC4-407C-B3F4-3A20CFD2675D}">
+    <sortState ref="A2:G24">
       <sortCondition ref="A1"/>
     </sortState>
   </autoFilter>

</xml_diff>